<commit_message>
Se corrigió las fechas de los hitos
</commit_message>
<xml_diff>
--- a/Desarrollo/SVL/SVL_C.xlsx
+++ b/Desarrollo/SVL/SVL_C.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Hoja 1'!$B$10:$H$36</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Hoja 1'!$B$10:$H$34</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="95">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -226,9 +226,6 @@
     <t>SVL_SBD.sql</t>
   </si>
   <si>
-    <t>Hito 3: Desarrollo de la Base de datos</t>
-  </si>
-  <si>
     <t>Desarrollo de Front-End</t>
   </si>
   <si>
@@ -250,7 +247,7 @@
     <t>Ramírez / Back-End Dev</t>
   </si>
   <si>
-    <t>Hito 4: Desarrollo Front-End y Back-End</t>
+    <t>Hito 3: Desarrollo y Pruebas</t>
   </si>
   <si>
     <t>Diseño de Casos de prueba</t>
@@ -277,9 +274,6 @@
     <t>Moreno / Tester</t>
   </si>
   <si>
-    <t>Hito 5: Pruebas de calidad QA</t>
-  </si>
-  <si>
     <t>Capacitación a usuarios de Brisol</t>
   </si>
   <si>
@@ -304,7 +298,7 @@
     <t>Ramírez / Back-End – Rojas / Front-End</t>
   </si>
   <si>
-    <t>Hito 6: Entrega final y capacitación</t>
+    <t>Hito 4: Despliegue</t>
   </si>
 </sst>
 </file>
@@ -536,11 +530,11 @@
     <xf borderId="3" fillId="2" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="7" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
@@ -1253,30 +1247,40 @@
       <c r="H26" s="24"/>
     </row>
     <row r="27">
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="36">
-        <v>45934.0</v>
-      </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="2"/>
+      <c r="C27" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="35">
+        <v>45935.0</v>
+      </c>
+      <c r="G27" s="35">
+        <v>45954.0</v>
+      </c>
+      <c r="H27" s="36">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" s="19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="F28" s="35">
         <v>45935.0</v>
@@ -1284,170 +1288,134 @@
       <c r="G28" s="35">
         <v>45954.0</v>
       </c>
-      <c r="H28" s="37">
+      <c r="H28" s="36"/>
+    </row>
+    <row r="29">
+      <c r="B29" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="37">
+        <v>45954.0</v>
+      </c>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" s="35">
+        <v>45955.0</v>
+      </c>
+      <c r="G30" s="35">
+        <v>45960.0</v>
+      </c>
+      <c r="H30" s="36">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="29">
-      <c r="B29" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="F29" s="35">
-        <v>45935.0</v>
-      </c>
-      <c r="G29" s="35">
-        <v>45954.0</v>
-      </c>
-      <c r="H29" s="37"/>
-    </row>
-    <row r="30">
-      <c r="B30" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" s="36">
-        <v>45954.0</v>
-      </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="2"/>
     </row>
     <row r="31">
       <c r="B31" s="25" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F31" s="35">
-        <v>45955.0</v>
-      </c>
-      <c r="G31" s="35">
-        <v>45960.0</v>
-      </c>
-      <c r="H31" s="37">
+        <v>45961.0</v>
+      </c>
+      <c r="G31" s="38">
+        <v>45967.0</v>
+      </c>
+      <c r="H31" s="36">
         <v>0.0</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" s="25" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="F32" s="35">
-        <v>45961.0</v>
+        <v>89</v>
+      </c>
+      <c r="F32" s="38">
+        <v>45968.0</v>
       </c>
       <c r="G32" s="38">
-        <v>45967.0</v>
-      </c>
-      <c r="H32" s="37">
+        <v>45973.0</v>
+      </c>
+      <c r="H32" s="36">
         <v>0.0</v>
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="36">
-        <v>45967.0</v>
-      </c>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="2"/>
+      <c r="B33" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" s="39">
+        <v>45974.0</v>
+      </c>
+      <c r="G33" s="39">
+        <v>45974.0</v>
+      </c>
+      <c r="H33" s="36">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="34">
-      <c r="B34" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="F34" s="38">
-        <v>45968.0</v>
-      </c>
-      <c r="G34" s="38">
-        <v>45973.0</v>
-      </c>
-      <c r="H34" s="37">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="B35" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="D35" s="25" t="s">
+      <c r="B34" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="F35" s="39">
+      <c r="C34" s="37">
         <v>45974.0</v>
       </c>
-      <c r="G35" s="39">
-        <v>45974.0</v>
-      </c>
-      <c r="H35" s="37">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="B36" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="2"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="$B$10:$H$36"/>
-  <mergeCells count="7">
+  <autoFilter ref="$B$10:$H$34"/>
+  <mergeCells count="5">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="C19:H19"/>
     <mergeCell ref="C25:H25"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C30:H30"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C34:H34"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>